<commit_message>
SP y VM Revisados
</commit_message>
<xml_diff>
--- a/Bitacora de activiades contabilidad pasada nro3.xlsx
+++ b/Bitacora de activiades contabilidad pasada nro3.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{01792D0C-941A-42C4-9B58-253AE23C24A2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Historico" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="123">
   <si>
     <t>Nro</t>
   </si>
@@ -372,12 +373,30 @@
   </si>
   <si>
     <t>Contabilidad</t>
+  </si>
+  <si>
+    <t>clsTipoPlan</t>
+  </si>
+  <si>
+    <t>preguntar si la tabla sera poblada desde BD</t>
+  </si>
+  <si>
+    <t>ctbTipoPlan</t>
+  </si>
+  <si>
+    <t>clsTipoPLanVM</t>
+  </si>
+  <si>
+    <t>Variables static</t>
+  </si>
+  <si>
+    <t>se pobla desde BD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,7 +414,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,6 +454,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -503,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -538,15 +563,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -565,11 +581,26 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -587,16 +618,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -689,6 +710,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -724,6 +762,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -899,15 +954,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:L325"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1883,14 +1938,68 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G30" s="4">
+        <v>43266</v>
+      </c>
+      <c r="H30" s="4">
+        <v>43266</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G31" s="4">
+        <v>43266</v>
+      </c>
+      <c r="H31" s="4">
+        <v>43266</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -3370,6 +3479,19 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{C7E5F826-5049-4106-95C8-BF4F1FB06DEB}">
+            <xm:f>'Valores columnas'!$I$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C6500"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFEB9C"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
           <x14:cfRule type="cellIs" priority="2" operator="equal" id="{80E41AE6-0BBD-44D4-BDBE-78982EED740E}">
             <xm:f>'Valores columnas'!$I$2</xm:f>
             <x14:dxf>
@@ -3383,38 +3505,25 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{C7E5F826-5049-4106-95C8-BF4F1FB06DEB}">
-            <xm:f>'Valores columnas'!$I$3</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C6500"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFEB9C"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
           <xm:sqref>D1:D1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'Valores columnas'!$A$2:$A$5</xm:f>
           </x14:formula1>
           <xm:sqref>I19:I1048576 I1:I17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'Valores columnas'!$G$2:$G$3</xm:f>
           </x14:formula1>
           <xm:sqref>B19:B1048576 B1:B17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>'Valores columnas'!$I$2:$I$4</xm:f>
           </x14:formula1>
@@ -3427,489 +3536,574 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" style="3" customWidth="1"/>
-    <col min="2" max="5" width="11.42578125" style="18"/>
-    <col min="6" max="6" width="17" style="19" customWidth="1"/>
-    <col min="7" max="9" width="11.42578125" style="19"/>
-    <col min="10" max="10" width="18.7109375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="1"/>
+    <col min="2" max="5" width="11.42578125" style="15"/>
+    <col min="6" max="6" width="17" style="16" customWidth="1"/>
+    <col min="7" max="9" width="11.42578125" style="16"/>
+    <col min="10" max="10" width="11.42578125" style="18"/>
+    <col min="11" max="11" width="18.7109375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="14" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" s="14"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="J8" s="1" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="K8" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="J9" s="1" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B11" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="I15" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="H16" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B16" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="H17" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="I17" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="J17" s="1" t="s">
+      <c r="B17" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="H18" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="B18" s="17"/>
+      <c r="C18" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3921,13 +4115,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>'Valores columnas'!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B1:E1048576</xm:sqref>
+          <xm:sqref>B1:E1048576 J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>'Valores columnas'!$C$2:$C$3</xm:f>
           </x14:formula1>
@@ -3940,7 +4134,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3980,7 +4174,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -4033,7 +4227,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>